<commit_message>
Inserido grafico de análise
Inseri o grafico comentado em aula com 2 eixos
está na planilha "planilha análises
</commit_message>
<xml_diff>
--- a/Analise redes.xlsx
+++ b/Analise redes.xlsx
@@ -454,11 +454,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="341030008"/>
-        <c:axId val="341025304"/>
+        <c:axId val="251977584"/>
+        <c:axId val="251977976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="341030008"/>
+        <c:axId val="251977584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -501,7 +501,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="341025304"/>
+        <c:crossAx val="251977976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -509,7 +509,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="341025304"/>
+        <c:axId val="251977976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -547,7 +547,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="341030008"/>
+        <c:crossAx val="251977584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -874,11 +874,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="282017072"/>
-        <c:axId val="282018640"/>
+        <c:axId val="251979152"/>
+        <c:axId val="251979544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="282017072"/>
+        <c:axId val="251979152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -921,7 +921,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="282018640"/>
+        <c:crossAx val="251979544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -929,7 +929,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="282018640"/>
+        <c:axId val="251979544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -967,7 +967,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="282017072"/>
+        <c:crossAx val="251979152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1289,11 +1289,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="341035496"/>
-        <c:axId val="341032360"/>
+        <c:axId val="251972880"/>
+        <c:axId val="253921352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="341035496"/>
+        <c:axId val="251972880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1336,7 +1336,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="341032360"/>
+        <c:crossAx val="253921352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1344,7 +1344,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="341032360"/>
+        <c:axId val="253921352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1800"/>
@@ -1383,7 +1383,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="341035496"/>
+        <c:crossAx val="251972880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1701,11 +1701,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="277753672"/>
-        <c:axId val="277750536"/>
+        <c:axId val="253923312"/>
+        <c:axId val="253922136"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="277753672"/>
+        <c:axId val="253923312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1748,7 +1748,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="277750536"/>
+        <c:crossAx val="253922136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1756,7 +1756,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="277750536"/>
+        <c:axId val="253922136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1794,7 +1794,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="277753672"/>
+        <c:crossAx val="253923312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1806,6 +1806,707 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>Análise</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" baseline="0"/>
+              <a:t> quanto a centralidade de Proximidade e de eficiência</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plan1!$D$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Proximidade</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Plan1!$E$21:$Q$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Plan1!$E$22:$Q$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>6.25E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.8799999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.5500000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.5500000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.3300000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.1199999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.3199999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.61E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.4000000000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.7999999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.8999999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.2000000000000001E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="274375656"/>
+        <c:axId val="274379968"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plan1!$D$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Eficiência</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.8284776902887138E-2"/>
+                  <c:y val="-5.7835739282589678E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Plan1!$E$21:$Q$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Plan1!$E$24:$Q$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.17</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="373744328"/>
+        <c:axId val="373743936"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="274375656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="274379968"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="274379968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="274375656"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="373743936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="373744328"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="373744328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="373743936"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.1438320209973754E-2"/>
+          <c:y val="0.87557815689705432"/>
+          <c:w val="0.90045669291338581"/>
+          <c:h val="0.10590332458442694"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2003,6 +2704,43 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="11">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent5"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3983,6 +4721,522 @@
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="322">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -4137,6 +5391,36 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>1994646</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>34739</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>358590</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>78441</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4405,8 +5689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:T27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4901,7 +6185,9 @@
     <row r="20" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
+      <c r="E20" s="3">
+        <v>0.33</v>
+      </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>

</xml_diff>

<commit_message>
adicionado graficos sobre as redes como imagens
adicionado graficos sobre as redes como imagens e planilha com os
graficos das redes geradas que foram utilizado no artigo
</commit_message>
<xml_diff>
--- a/Analise redes.xlsx
+++ b/Analise redes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20220" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>Numero</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t xml:space="preserve">na grande maioria dos casos pode-se observar que quanto maior o grau medio, de redes com o mesmo numero de nós, menor será a centralidade de intermediação </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -349,10 +352,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Plan1!$E$21:$Q$21</c:f>
+              <c:f>Plan1!$E$21:$P$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -388,19 +391,16 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Plan1!$E$22:$Q$22</c:f>
+              <c:f>Plan1!$E$22:$P$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>6.25E-2</c:v>
                 </c:pt>
@@ -435,9 +435,6 @@
                   <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.8999999999999998E-3</c:v>
-                </c:pt>
-                <c:pt idx="12">
                   <c:v>2.2000000000000001E-3</c:v>
                 </c:pt>
               </c:numCache>
@@ -454,11 +451,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="251977584"/>
-        <c:axId val="251977976"/>
+        <c:axId val="246989424"/>
+        <c:axId val="246990208"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="251977584"/>
+        <c:axId val="246989424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -501,7 +498,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="251977976"/>
+        <c:crossAx val="246990208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -509,7 +506,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="251977976"/>
+        <c:axId val="246990208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -547,7 +544,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="251977584"/>
+        <c:crossAx val="246989424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -603,10 +600,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="105"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="5"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -699,9 +696,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent6">
-                <a:lumMod val="50000"/>
-              </a:schemeClr>
+              <a:schemeClr val="accent3"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -769,10 +764,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Plan1!$E$21:$Q$21</c:f>
+              <c:f>Plan1!$E$21:$P$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -808,19 +803,16 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Plan1!$E$24:$Q$24</c:f>
+              <c:f>Plan1!$E$24:$P$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.33</c:v>
                 </c:pt>
@@ -855,9 +847,6 @@
                   <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.11</c:v>
-                </c:pt>
-                <c:pt idx="12">
                   <c:v>0.11</c:v>
                 </c:pt>
               </c:numCache>
@@ -874,11 +863,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="251979152"/>
-        <c:axId val="251979544"/>
+        <c:axId val="249835416"/>
+        <c:axId val="249831104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="251979152"/>
+        <c:axId val="249835416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -921,7 +910,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="251979544"/>
+        <c:crossAx val="249831104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -929,7 +918,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="251979544"/>
+        <c:axId val="249831104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -967,7 +956,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="251979152"/>
+        <c:crossAx val="249835416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1023,10 +1012,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="101"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="1"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -1116,7 +1105,9 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="002060"/>
+              <a:schemeClr val="dk1">
+                <a:tint val="88500"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1184,10 +1175,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Plan1!$E$21:$Q$21</c:f>
+              <c:f>Plan1!$E$21:$P$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1223,19 +1214,16 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Plan1!$E$25:$Q$25</c:f>
+              <c:f>Plan1!$E$25:$P$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>12.58</c:v>
                 </c:pt>
@@ -1270,9 +1258,6 @@
                   <c:v>631.41999999999996</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1034.95</c:v>
-                </c:pt>
-                <c:pt idx="12">
                   <c:v>1720.56</c:v>
                 </c:pt>
               </c:numCache>
@@ -1289,11 +1274,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="251972880"/>
-        <c:axId val="253921352"/>
+        <c:axId val="249837376"/>
+        <c:axId val="249831888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="251972880"/>
+        <c:axId val="249837376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1336,7 +1321,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="253921352"/>
+        <c:crossAx val="249831888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1344,7 +1329,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="253921352"/>
+        <c:axId val="249831888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1800"/>
@@ -1383,7 +1368,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="251972880"/>
+        <c:crossAx val="249837376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1596,10 +1581,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Plan1!$E$21:$Q$21</c:f>
+              <c:f>Plan1!$E$21:$P$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1635,19 +1620,16 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Plan1!$E$26:$Q$26</c:f>
+              <c:f>Plan1!$E$26:$P$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.33</c:v>
                 </c:pt>
@@ -1682,9 +1664,6 @@
                   <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.0000000000000007E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
                   <c:v>0.06</c:v>
                 </c:pt>
               </c:numCache>
@@ -1701,11 +1680,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="253923312"/>
-        <c:axId val="253922136"/>
+        <c:axId val="249834240"/>
+        <c:axId val="249838160"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="253923312"/>
+        <c:axId val="249834240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1748,7 +1727,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="253922136"/>
+        <c:crossAx val="249838160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1756,7 +1735,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="253922136"/>
+        <c:axId val="249838160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1794,7 +1773,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="253923312"/>
+        <c:crossAx val="249834240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1850,10 +1829,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="101"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="1"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -1878,13 +1857,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pt-BR"/>
-              <a:t>Análise</a:t>
+              <a:t>Análise quanto a centralidade de Proximidade e de Eficiência</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="pt-BR" baseline="0"/>
-              <a:t> quanto a centralidade de Proximidade e de eficiência</a:t>
-            </a:r>
-            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1941,7 +1915,9 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="dk1">
+                <a:tint val="88500"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1951,10 +1927,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Plan1!$E$21:$Q$21</c:f>
+              <c:f>Plan1!$E$21:$P$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1990,19 +1966,16 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Plan1!$E$22:$Q$22</c:f>
+              <c:f>Plan1!$E$22:$P$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>6.25E-2</c:v>
                 </c:pt>
@@ -2037,9 +2010,6 @@
                   <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.8999999999999998E-3</c:v>
-                </c:pt>
-                <c:pt idx="12">
                   <c:v>2.2000000000000001E-3</c:v>
                 </c:pt>
               </c:numCache>
@@ -2055,8 +2025,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="274375656"/>
-        <c:axId val="274379968"/>
+        <c:axId val="249836592"/>
+        <c:axId val="249836200"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2078,7 +2048,9 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="dk1">
+                  <a:tint val="55000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2169,10 +2141,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Plan1!$E$21:$Q$21</c:f>
+              <c:f>Plan1!$E$21:$P$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2208,19 +2180,16 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Plan1!$E$24:$Q$24</c:f>
+              <c:f>Plan1!$E$24:$P$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.33</c:v>
                 </c:pt>
@@ -2255,9 +2224,6 @@
                   <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.11</c:v>
-                </c:pt>
-                <c:pt idx="12">
                   <c:v>0.11</c:v>
                 </c:pt>
               </c:numCache>
@@ -2275,11 +2241,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="373744328"/>
-        <c:axId val="373743936"/>
+        <c:axId val="249833456"/>
+        <c:axId val="249833064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="274375656"/>
+        <c:axId val="249836592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2322,7 +2288,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="274379968"/>
+        <c:crossAx val="249836200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2330,7 +2296,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="274379968"/>
+        <c:axId val="249836200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2381,12 +2347,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="274375656"/>
+        <c:crossAx val="249836592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="373743936"/>
+        <c:axId val="249833064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2437,12 +2403,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="373744328"/>
+        <c:crossAx val="249833456"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="373744328"/>
+        <c:axId val="249833456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2452,7 +2418,8 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="373743936"/>
+        <c:crossAx val="249833064"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2468,16 +2435,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="4.1438320209973754E-2"/>
-          <c:y val="0.87557815689705432"/>
-          <c:w val="0.90045669291338581"/>
-          <c:h val="0.10590332458442694"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2585,81 +2543,34 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="16">
   <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
 </cs:colorStyle>
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="20">
+  <a:schemeClr val="dk1"/>
   <cs:variation>
-    <a:lumMod val="60000"/>
+    <a:tint val="88500"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
+    <a:tint val="55000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="80000"/>
+    <a:tint val="75000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
+    <a:tint val="98500"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="50000"/>
+    <a:tint val="30000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
+    <a:tint val="60000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
+    <a:tint val="80000"/>
   </cs:variation>
 </cs:colorStyle>
 </file>
@@ -2705,38 +2616,28 @@
 </file>
 
 <file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="11">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent5"/>
-  <cs:variation/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="20">
+  <a:schemeClr val="dk1"/>
   <cs:variation>
-    <a:lumMod val="60000"/>
+    <a:tint val="88500"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
+    <a:tint val="55000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="80000"/>
+    <a:tint val="75000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
+    <a:tint val="98500"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="50000"/>
+    <a:tint val="30000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
+    <a:tint val="60000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
+    <a:tint val="80000"/>
   </cs:variation>
 </cs:colorStyle>
 </file>
@@ -5364,15 +5265,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>467446</xdr:colOff>
+      <xdr:colOff>467445</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>187898</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>448077</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>91109</xdr:colOff>
       <xdr:row>60</xdr:row>
-      <xdr:rowOff>73598</xdr:rowOff>
+      <xdr:rowOff>74543</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5689,8 +5590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:T27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="K24" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="AD34" sqref="AD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6115,66 +6016,42 @@
         <v>12</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E15" s="3">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="F15" s="3">
-        <v>97</v>
+        <v>171</v>
       </c>
       <c r="G15" s="3">
-        <v>2.59</v>
+        <v>3.42</v>
       </c>
       <c r="H15" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I15" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>0.06</v>
       </c>
       <c r="J15" s="3">
         <v>0.11</v>
       </c>
       <c r="K15" s="3">
-        <v>2.8999999999999998E-3</v>
+        <v>2.2000000000000001E-3</v>
       </c>
       <c r="L15" s="3">
-        <v>1034.95</v>
+        <v>1720.56</v>
       </c>
     </row>
     <row r="16" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C16" s="3">
-        <v>13</v>
+      <c r="C16" t="s">
+        <v>27</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" s="3">
-        <v>100</v>
-      </c>
-      <c r="F16" s="3">
-        <v>171</v>
-      </c>
-      <c r="G16" s="3">
-        <v>3.42</v>
-      </c>
-      <c r="H16" s="3">
-        <v>6</v>
-      </c>
-      <c r="I16" s="3">
-        <v>0.06</v>
-      </c>
-      <c r="J16" s="3">
-        <v>0.11</v>
-      </c>
-      <c r="K16" s="3">
-        <v>2.2000000000000001E-3</v>
-      </c>
-      <c r="L16" s="3">
-        <v>1720.56</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="17" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
@@ -6182,7 +6059,39 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="20" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C18" s="3">
+        <v>12</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="3">
+        <v>75</v>
+      </c>
+      <c r="F18" s="3">
+        <v>97</v>
+      </c>
+      <c r="G18" s="3">
+        <v>2.59</v>
+      </c>
+      <c r="H18" s="3">
+        <v>5</v>
+      </c>
+      <c r="I18" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J18" s="3">
+        <v>0.11</v>
+      </c>
+      <c r="K18" s="3">
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="L18" s="3">
+        <v>1034.95</v>
+      </c>
+    </row>
+    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3">
@@ -6196,7 +6105,7 @@
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
     </row>
-    <row r="21" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C21" s="3"/>
       <c r="D21" s="2" t="s">
         <v>23</v>
@@ -6237,11 +6146,8 @@
       <c r="P21" s="3">
         <v>12</v>
       </c>
-      <c r="Q21" s="3">
-        <v>13</v>
-      </c>
     </row>
-    <row r="22" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C22" s="3"/>
       <c r="D22" s="2" t="s">
         <v>4</v>
@@ -6280,13 +6186,10 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="P22" s="3">
-        <v>2.8999999999999998E-3</v>
-      </c>
-      <c r="Q22" s="3">
         <v>2.2000000000000001E-3</v>
       </c>
     </row>
-    <row r="23" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C23" s="3"/>
       <c r="D23" s="2" t="s">
         <v>22</v>
@@ -6325,13 +6228,10 @@
         <v>56</v>
       </c>
       <c r="P23" s="3">
-        <v>75</v>
-      </c>
-      <c r="Q23" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C24" s="3"/>
       <c r="D24" s="2" t="s">
         <v>3</v>
@@ -6372,11 +6272,8 @@
       <c r="P24" s="3">
         <v>0.11</v>
       </c>
-      <c r="Q24" s="3">
-        <v>0.11</v>
-      </c>
     </row>
-    <row r="25" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C25" s="3"/>
       <c r="D25" s="2" t="s">
         <v>8</v>
@@ -6415,13 +6312,10 @@
         <v>631.41999999999996</v>
       </c>
       <c r="P25" s="3">
-        <v>1034.95</v>
-      </c>
-      <c r="Q25" s="3">
         <v>1720.56</v>
       </c>
     </row>
-    <row r="26" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C26" s="3"/>
       <c r="D26" s="2" t="s">
         <v>7</v>
@@ -6460,13 +6354,10 @@
         <v>0.05</v>
       </c>
       <c r="P26" s="3">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="Q26" s="3">
         <v>0.06</v>
       </c>
     </row>
-    <row r="27" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>

</xml_diff>